<commit_message>
MTPO - Don1 phase 1 Lua script modification
</commit_message>
<xml_diff>
--- a/MTPO/MTPOTrainingStats.xlsx
+++ b/MTPO/MTPOTrainingStats.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="14220" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Hippo" sheetId="4" r:id="rId1"/>
-    <sheet name="Tiger" sheetId="1" r:id="rId2"/>
+    <sheet name="Don1-Phase1" sheetId="5" r:id="rId1"/>
+    <sheet name="Hippo" sheetId="4" r:id="rId2"/>
+    <sheet name="Tiger" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="14">
   <si>
     <t>Perfects</t>
   </si>
@@ -595,7 +596,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:H7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,13 +631,13 @@
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A4" s="13">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B4" s="21">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C4" s="15">
-        <v>430</v>
+        <v>162</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>0</v>
@@ -648,42 +649,30 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A5" s="13">
-        <v>13</v>
-      </c>
-      <c r="B5" s="21">
-        <v>140</v>
-      </c>
-      <c r="C5" s="15">
-        <v>451</v>
-      </c>
+      <c r="A5" s="13"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="15"/>
       <c r="F5" s="13"/>
       <c r="G5" s="21"/>
       <c r="H5" s="15"/>
       <c r="J5">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="13">
-        <v>17</v>
-      </c>
-      <c r="B6" s="14">
-        <v>117</v>
-      </c>
-      <c r="C6" s="15">
-        <v>283</v>
-      </c>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
       <c r="F6" s="13"/>
       <c r="G6" s="21"/>
       <c r="H6" s="15"/>
       <c r="J6">
         <f>SUM(J3:J5)</f>
-        <v>117</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -745,15 +734,15 @@
     <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A14" s="18">
         <f>SUM(A4:A13)</f>
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B14" s="19">
         <f>SUM(B4:B13)</f>
-        <v>368</v>
+        <v>83</v>
       </c>
       <c r="C14" s="20">
         <f>SUM(C4:C13)</f>
-        <v>1164</v>
+        <v>162</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="9"/>
@@ -786,14 +775,14 @@
     <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="3">
         <f>ROUND(A14/B14*100,1)</f>
-        <v>9.8000000000000007</v>
+        <v>20.5</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="7">
         <f>ROUND(C14/B14,2)</f>
-        <v>3.16</v>
+        <v>1.95</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>6</v>
@@ -831,7 +820,7 @@
     <row r="20" spans="1:9">
       <c r="A20">
         <f>ROUND(((A17/100)*(A17/100)) * 100, 2)</f>
-        <v>0.96</v>
+        <v>4.2</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -843,7 +832,7 @@
     <row r="21" spans="1:9">
       <c r="A21">
         <f>ROUND(((A17/100)*(A17/100)*(A17/100)) * 100, 2)</f>
-        <v>0.09</v>
+        <v>0.86</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -855,7 +844,7 @@
     <row r="22" spans="1:9">
       <c r="A22">
         <f>ROUND(((A17/100)*(A17/100)*(A17/100) * (A17/100)) * 100, 2)</f>
-        <v>0.01</v>
+        <v>0.18</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -871,6 +860,286 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="18.75">
+      <c r="A1" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A4" s="13">
+        <v>6</v>
+      </c>
+      <c r="B4" s="21">
+        <v>111</v>
+      </c>
+      <c r="C4" s="15">
+        <v>430</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A5" s="13">
+        <v>13</v>
+      </c>
+      <c r="B5" s="21">
+        <v>140</v>
+      </c>
+      <c r="C5" s="15">
+        <v>451</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="15"/>
+      <c r="J5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13">
+        <v>17</v>
+      </c>
+      <c r="B6" s="14">
+        <v>117</v>
+      </c>
+      <c r="C6" s="15">
+        <v>283</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="15"/>
+      <c r="J6">
+        <f>SUM(J3:J5)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="13"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="15"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="15"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="15"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="15"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="15"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="15"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="17"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A14" s="18">
+        <f>SUM(A4:A13)</f>
+        <v>36</v>
+      </c>
+      <c r="B14" s="19">
+        <f>SUM(B4:B13)</f>
+        <v>368</v>
+      </c>
+      <c r="C14" s="20">
+        <f>SUM(C4:C13)</f>
+        <v>1164</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+      <c r="F15" s="18">
+        <f>SUM(F5:F14)</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="19">
+        <f>SUM(G5:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
+        <f>SUM(H5:H14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A17" s="3">
+        <f>ROUND(A14/B14*100,1)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7">
+        <f>ROUND(C14/B14,2)</f>
+        <v>3.16</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+      <c r="F18" s="3" t="e">
+        <f>ROUND(F15/G15*100,1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7" t="e">
+        <f>ROUND(H15/G15,2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <f>ROUND(((A17/100)*(A17/100)) * 100, 2)</f>
+        <v>0.96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <f>ROUND(((A17/100)*(A17/100)*(A17/100)) * 100, 2)</f>
+        <v>0.09</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <f>ROUND(((A17/100)*(A17/100)*(A17/100) * (A17/100)) * 100, 2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J22"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add GB Tom and Jerry project that I started in 2007 but forgot about until now.
</commit_message>
<xml_diff>
--- a/MTPO/MTPOTrainingStats.xlsx
+++ b/MTPO/MTPOTrainingStats.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="14220" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Don1-Phase1" sheetId="5" r:id="rId1"/>
-    <sheet name="Hippo" sheetId="4" r:id="rId2"/>
-    <sheet name="Tiger" sheetId="1" r:id="rId3"/>
+    <sheet name="Tiger" sheetId="1" r:id="rId1"/>
+    <sheet name="Don1-Phase1" sheetId="5" r:id="rId2"/>
+    <sheet name="Hippo" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -596,7 +596,293 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="23" customFormat="1" ht="18.75">
+      <c r="A1" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A4" s="13">
+        <v>89</v>
+      </c>
+      <c r="B4" s="21">
+        <v>184</v>
+      </c>
+      <c r="C4" s="15">
+        <v>139</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="F5" s="13">
+        <v>970</v>
+      </c>
+      <c r="G5" s="21">
+        <v>2266</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1689</v>
+      </c>
+      <c r="J5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="F6" s="13">
+        <v>70</v>
+      </c>
+      <c r="G6" s="21">
+        <v>268</v>
+      </c>
+      <c r="H6" s="15">
+        <v>270</v>
+      </c>
+      <c r="J6">
+        <f>SUM(J3:J5)</f>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="13"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="15"/>
+      <c r="F7" s="13">
+        <v>54</v>
+      </c>
+      <c r="G7" s="14">
+        <v>171</v>
+      </c>
+      <c r="H7" s="15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="15"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="15"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="15"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="15"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="15"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A13" s="16"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="17"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A14" s="18">
+        <f>SUM(A4:A13)</f>
+        <v>89</v>
+      </c>
+      <c r="B14" s="19">
+        <f>SUM(B4:B13)</f>
+        <v>184</v>
+      </c>
+      <c r="C14" s="20">
+        <f>SUM(C4:C13)</f>
+        <v>139</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+      <c r="F15" s="18">
+        <f>SUM(F5:F14)</f>
+        <v>1094</v>
+      </c>
+      <c r="G15" s="19">
+        <f>SUM(G5:G14)</f>
+        <v>2705</v>
+      </c>
+      <c r="H15" s="20">
+        <f>SUM(H5:H14)</f>
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A17" s="3">
+        <f>ROUND(A14/B14*100,1)</f>
+        <v>48.4</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7">
+        <f>ROUND(C14/B14,2)</f>
+        <v>0.76</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+      <c r="F18" s="3">
+        <f>ROUND(F15/G15*100,1)</f>
+        <v>40.4</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="7">
+        <f>ROUND(H15/G15,2)</f>
+        <v>0.78</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <f>ROUND(((A17/100)*(A17/100)) * 100, 2)</f>
+        <v>23.43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <f>ROUND(((A17/100)*(A17/100)*(A17/100)) * 100, 2)</f>
+        <v>11.34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <f>ROUND(((A17/100)*(A17/100)*(A17/100) * (A17/100)) * 100, 2)</f>
+        <v>5.49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -859,7 +1145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J22"/>
   <sheetViews>
@@ -1137,326 +1423,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1" ht="18.75">
-      <c r="A1" s="23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A4" s="13">
-        <v>75</v>
-      </c>
-      <c r="B4" s="21">
-        <v>199</v>
-      </c>
-      <c r="C4" s="15">
-        <v>158</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A5" s="13">
-        <v>45</v>
-      </c>
-      <c r="B5" s="14">
-        <v>123</v>
-      </c>
-      <c r="C5" s="15">
-        <v>78</v>
-      </c>
-      <c r="F5" s="13">
-        <v>354</v>
-      </c>
-      <c r="G5" s="21">
-        <v>835</v>
-      </c>
-      <c r="H5" s="15">
-        <v>685</v>
-      </c>
-      <c r="J5">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="13">
-        <v>69</v>
-      </c>
-      <c r="B6" s="14">
-        <v>240</v>
-      </c>
-      <c r="C6" s="15">
-        <v>171</v>
-      </c>
-      <c r="F6" s="13">
-        <v>55</v>
-      </c>
-      <c r="G6" s="21">
-        <v>115</v>
-      </c>
-      <c r="H6" s="15">
-        <v>83</v>
-      </c>
-      <c r="J6">
-        <f>SUM(J3:J5)</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="13"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="15"/>
-      <c r="F7" s="13">
-        <v>98</v>
-      </c>
-      <c r="G7" s="21">
-        <v>194</v>
-      </c>
-      <c r="H7" s="15">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="13"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="15"/>
-      <c r="F8" s="13">
-        <v>19</v>
-      </c>
-      <c r="G8" s="14">
-        <v>50</v>
-      </c>
-      <c r="H8" s="15">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="13"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="15"/>
-      <c r="F9" s="13">
-        <v>143</v>
-      </c>
-      <c r="G9" s="14">
-        <v>300</v>
-      </c>
-      <c r="H9" s="15">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="13"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="15"/>
-      <c r="F10" s="13">
-        <v>81</v>
-      </c>
-      <c r="G10" s="21">
-        <v>150</v>
-      </c>
-      <c r="H10" s="15">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="15"/>
-      <c r="F11" s="13">
-        <v>31</v>
-      </c>
-      <c r="G11" s="21">
-        <v>60</v>
-      </c>
-      <c r="H11" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="13"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="15"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="17"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A14" s="18">
-        <f>SUM(A4:A13)</f>
-        <v>189</v>
-      </c>
-      <c r="B14" s="19">
-        <f>SUM(B4:B13)</f>
-        <v>562</v>
-      </c>
-      <c r="C14" s="20">
-        <f>SUM(C4:C13)</f>
-        <v>407</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="17"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="F15" s="18">
-        <f>SUM(F5:F14)</f>
-        <v>781</v>
-      </c>
-      <c r="G15" s="19">
-        <f>SUM(G5:G14)</f>
-        <v>1704</v>
-      </c>
-      <c r="H15" s="20">
-        <f>SUM(H5:H14)</f>
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A17" s="3">
-        <f>ROUND(A14/B14*100,1)</f>
-        <v>33.6</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="7">
-        <f>ROUND(C14/B14,2)</f>
-        <v>0.72</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="F18" s="3">
-        <f>ROUND(F15/G15*100,1)</f>
-        <v>45.8</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="7">
-        <f>ROUND(H15/G15,2)</f>
-        <v>0.75</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20">
-        <f>ROUND(((A17/100)*(A17/100)) * 100, 2)</f>
-        <v>11.29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21">
-        <f>ROUND(((A17/100)*(A17/100)*(A17/100)) * 100, 2)</f>
-        <v>3.79</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22">
-        <f>ROUND(((A17/100)*(A17/100)*(A17/100) * (A17/100)) * 100, 2)</f>
-        <v>1.27</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>